<commit_message>
Updated Template structure with embedded Page Layout and Print settings
</commit_message>
<xml_diff>
--- a/generated.xlsx
+++ b/generated.xlsx
@@ -23,10 +23,29 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>DIAS</t>
+  </si>
+  <si>
+    <t>DOOR</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -42,7 +61,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -265,11 +284,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -289,6 +334,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -572,167 +641,279 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B11:N21"/>
+  <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="11" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B12" s="1"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="3"/>
-    </row>
-    <row r="13" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="4"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="6"/>
-    </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B14" s="4"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="11"/>
-      <c r="L14" s="12"/>
-      <c r="M14" s="13"/>
-      <c r="N14" s="6"/>
-    </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B15" s="4"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="10"/>
-      <c r="M15" s="15"/>
-      <c r="N15" s="6"/>
-    </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B16" s="4"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="10"/>
-      <c r="M16" s="15"/>
-      <c r="N16" s="6"/>
-    </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B17" s="4"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="10"/>
-      <c r="M17" s="15"/>
-      <c r="N17" s="6"/>
-    </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B18" s="4"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="14"/>
-      <c r="L18" s="10"/>
-      <c r="M18" s="15"/>
-      <c r="N18" s="6"/>
-    </row>
-    <row r="19" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="4"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="18"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="16"/>
-      <c r="L19" s="17"/>
-      <c r="M19" s="18"/>
-      <c r="N19" s="6"/>
-    </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B20" s="4"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="5"/>
-      <c r="N20" s="6"/>
-    </row>
-    <row r="21" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="7"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="8"/>
-      <c r="K21" s="8"/>
-      <c r="L21" s="8"/>
-      <c r="M21" s="8"/>
-      <c r="N21" s="9"/>
+    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="20"/>
+    </row>
+    <row r="2" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="3"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="22"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="6"/>
+    </row>
+    <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="6"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="6"/>
+    </row>
+    <row r="6" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="6"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="6"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="6"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="6"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="6"/>
+      <c r="O10" s="5"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="6"/>
+      <c r="O11" s="5"/>
+    </row>
+    <row r="12" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="4"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="18"/>
+      <c r="M12" s="6"/>
+      <c r="O12" s="5"/>
+    </row>
+    <row r="13" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="7"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="9"/>
+      <c r="O13" s="5"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="5"/>
+      <c r="O14" s="5"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="5"/>
+      <c r="O15" s="5"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="5"/>
+      <c r="O16" s="5"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="5"/>
+      <c r="O17" s="5"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="5"/>
+      <c r="O18" s="5"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="5"/>
+      <c r="O19" s="5"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="5"/>
+      <c r="O20" s="5"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+      <c r="O22" s="5"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="F3:H4"/>
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
+  <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" fitToHeight="0" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;G</oddHeader>
+    <oddFooter>&amp;LDepartment of Computer Science &amp; Engineering&amp;RSeating arrangement generated by ISMGen.</oddFooter>
+  </headerFooter>
+  <legacyDrawingHF r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>